<commit_message>
Added questions about the data
There is so much good here. Diarmuid has good questions to pose about the data:
• Are there repeats in the data?
• Will this analysis need to be repeated or is it a one time deal?
• Will I need to explain what I am doing to someone else?
• If there are repeats, how are the repeats to be handled?

Also, he did an excellent job of coming up with a good data check strategy. This needs to be followed up. This may be the best approach to ensuring workbook quality and accuracy.
</commit_message>
<xml_diff>
--- a/ExcelExpertsChallenge-Diarmuid.xlsx
+++ b/ExcelExpertsChallenge-Diarmuid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{E81D9676-1A6B-4AF7-8FA4-8C9815FB05C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC73B020-E408-4364-8A0A-3871F5A6D09A}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{E81D9676-1A6B-4AF7-8FA4-8C9815FB05C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89B10062-365C-4F6D-B266-913E7EE14A37}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="7140" yWindow="45" windowWidth="21600" windowHeight="11385" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="69">
   <si>
     <t>FROM:</t>
   </si>
@@ -267,6 +267,27 @@
   </si>
   <si>
     <t>Cross-Check</t>
+  </si>
+  <si>
+    <t>Masterful use of wraprows</t>
+  </si>
+  <si>
+    <t>Questions to Ask When Analyzing Data</t>
+  </si>
+  <si>
+    <t>HSTACK to fill in multiple adjacent cells</t>
+  </si>
+  <si>
+    <t>Is this one time or will it repeat?</t>
+  </si>
+  <si>
+    <t>Repeats in the data?</t>
+  </si>
+  <si>
+    <t>Will I have to explain it to anyone?</t>
+  </si>
+  <si>
+    <t>If there are repeats, how should the repeats be handled? In this case, the repeats are handled by taking the hightest score.</t>
   </si>
 </sst>
 </file>
@@ -459,7 +480,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -471,6 +492,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -908,6 +930,50 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>832380</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1F3494A-8B8C-49C9-75B2-CD27D3DA09E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="612321" y="10423071"/>
+          <a:ext cx="5540452" cy="1959429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -958,10 +1024,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1043,7 +1105,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1395,8 +1457,8 @@
   </sheetPr>
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1430,6 +1492,9 @@
       <c r="D1" s="9" t="s">
         <v>55</v>
       </c>
+      <c r="I1" s="11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1452,10 +1517,30 @@
       <c r="E3" t="s">
         <v>60</v>
       </c>
+      <c r="I3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" x14ac:dyDescent="0.25">

</xml_diff>